<commit_message>
changed structure from tests
</commit_message>
<xml_diff>
--- a/Documentation/Time Management/Zeitaufzeichnung_Gerhold.xlsx
+++ b/Documentation/Time Management/Zeitaufzeichnung_Gerhold.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23007"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23014"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni\4. Semester\Software Engineering\PS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{627FAE6C-9D25-4EA1-8779-39584005F423}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{355F3C3D-21C4-48A8-9583-1CC63D254E10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6E71D473-8E99-584F-9CE7-0EC5B1B78532}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="56">
   <si>
     <t>.</t>
   </si>
@@ -183,6 +183,15 @@
   </si>
   <si>
     <t>Teambesprechung (1 Stunde weniger)</t>
+  </si>
+  <si>
+    <t>Department Statistiken auf Teambasis implementiert</t>
+  </si>
+  <si>
+    <t>Tests und Statistiken implementiert</t>
+  </si>
+  <si>
+    <t>Tests und code clean up</t>
   </si>
   <si>
     <t>ID</t>
@@ -612,11 +621,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F855F84B-A166-7442-8B83-EBB2C6A67214}">
-  <dimension ref="A1:D1007"/>
+  <dimension ref="A1:D1008"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C28" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="D50" sqref="D50"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C40" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="B56" sqref="B56"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
     </sheetView>
@@ -1330,29 +1339,74 @@
       </c>
     </row>
     <row r="51" spans="1:4">
-      <c r="A51" s="8"/>
-      <c r="B51" s="7"/>
-      <c r="D51" s="3"/>
+      <c r="A51" s="8">
+        <v>43994</v>
+      </c>
+      <c r="B51" s="7">
+        <v>6.25E-2</v>
+      </c>
+      <c r="C51" t="s">
+        <v>15</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="52" spans="1:4">
-      <c r="A52" s="8"/>
-      <c r="B52" s="7"/>
-      <c r="D52" s="3"/>
+      <c r="A52" s="8">
+        <v>43997</v>
+      </c>
+      <c r="B52" s="7">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C52" t="s">
+        <v>4</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="53" spans="1:4">
-      <c r="A53" s="8"/>
-      <c r="B53" s="7"/>
-      <c r="D53" s="3"/>
+      <c r="A53" s="8">
+        <v>43997</v>
+      </c>
+      <c r="B53" s="7">
+        <v>6.25E-2</v>
+      </c>
+      <c r="C53" t="s">
+        <v>15</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="54" spans="1:4">
-      <c r="A54" s="8"/>
-      <c r="B54" s="7"/>
-      <c r="D54" s="3"/>
+      <c r="A54" s="8">
+        <v>44000</v>
+      </c>
+      <c r="B54" s="7">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C54" t="s">
+        <v>15</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="55" spans="1:4">
-      <c r="A55" s="8"/>
-      <c r="B55" s="7"/>
-      <c r="D55" s="3"/>
+      <c r="A55" s="8">
+        <v>44000</v>
+      </c>
+      <c r="B55" s="7">
+        <v>0.125</v>
+      </c>
+      <c r="C55" t="s">
+        <v>9</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="8"/>
@@ -6105,9 +6159,14 @@
       <c r="D1005" s="3"/>
     </row>
     <row r="1006" spans="1:4">
-      <c r="A1006" s="2"/>
-    </row>
-    <row r="1007" spans="1:4" ht="15.75"/>
+      <c r="A1006" s="8"/>
+      <c r="B1006" s="7"/>
+      <c r="D1006" s="3"/>
+    </row>
+    <row r="1007" spans="1:4">
+      <c r="A1007" s="2"/>
+    </row>
+    <row r="1008" spans="1:4" ht="15.75"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -6118,7 +6177,7 @@
           <x14:formula1>
             <xm:f>Tätigkeiten!$B$2:$B$12</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C1005</xm:sqref>
+          <xm:sqref>C2:C1006</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -6139,10 +6198,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -6174,7 +6233,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -6182,7 +6241,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -6198,7 +6257,7 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -6214,7 +6273,7 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -6222,7 +6281,7 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:2">

</xml_diff>